<commit_message>
updated results with correct font
</commit_message>
<xml_diff>
--- a/results/AYTO S3/results.xlsx
+++ b/results/AYTO S3/results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 00" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 02" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 04" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 06" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 08" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 09" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 10" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 12" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Episode 14" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Episode 00" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Episode 02" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Episode 04" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Episode 06" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Episode 08" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Episode 09" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Episode 10" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Episode 12" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Episode 14" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>